<commit_message>
added commission test data
</commit_message>
<xml_diff>
--- a/Timesheet-evaluation.xlsx
+++ b/Timesheet-evaluation.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="81">
   <si>
     <t xml:space="preserve">ETU001844</t>
   </si>
@@ -119,36 +119,6 @@
     <t xml:space="preserve">reset db function</t>
   </si>
   <si>
-    <t xml:space="preserve">model Region</t>
-  </si>
-  <si>
-    <t xml:space="preserve">model Proprietaire</t>
-  </si>
-  <si>
-    <t xml:space="preserve">model TypeBien</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Model TypeBienCommission</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Model VtypeBien</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Model Client</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Model Location</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Model Payement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Model VlocationPayementReste</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Model VlocationCommission</t>
-  </si>
-  <si>
     <t xml:space="preserve">proto Admin</t>
   </si>
   <si>
@@ -267,6 +237,9 @@
   </si>
   <si>
     <t xml:space="preserve">location imports</t>
+  </si>
+  <si>
+    <t xml:space="preserve">commission imports</t>
   </si>
   <si>
     <t xml:space="preserve">Service Import</t>
@@ -529,7 +502,7 @@
   <dimension ref="A1:H1003"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A97" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F24" activeCellId="0" sqref="F24"/>
+      <selection pane="topLeft" activeCell="H111" activeCellId="0" sqref="H111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.22265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1003,231 +976,111 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>32</v>
-      </c>
+      <c r="A23" s="6"/>
+      <c r="B23" s="6"/>
       <c r="C23" s="7"/>
       <c r="D23" s="8"/>
-      <c r="E23" s="8" t="n">
-        <v>2</v>
-      </c>
+      <c r="E23" s="8"/>
       <c r="F23" s="8"/>
-      <c r="G23" s="8" t="n">
-        <f aca="false">E23-F23</f>
-        <v>2</v>
-      </c>
-      <c r="H23" s="9" t="n">
-        <f aca="false">(F23/(F23+G23))</f>
-        <v>0</v>
-      </c>
+      <c r="G23" s="8"/>
+      <c r="H23" s="9"/>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>33</v>
-      </c>
+      <c r="A24" s="6"/>
+      <c r="B24" s="6"/>
       <c r="C24" s="7"/>
       <c r="D24" s="8"/>
-      <c r="E24" s="8" t="n">
-        <v>2</v>
-      </c>
+      <c r="E24" s="8"/>
       <c r="F24" s="8"/>
-      <c r="G24" s="8" t="n">
-        <f aca="false">E24-F24</f>
-        <v>2</v>
-      </c>
-      <c r="H24" s="9" t="n">
-        <f aca="false">(F24/(F24+G24))</f>
-        <v>0</v>
-      </c>
+      <c r="G24" s="8"/>
+      <c r="H24" s="9"/>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>34</v>
-      </c>
+      <c r="A25" s="6"/>
+      <c r="B25" s="6"/>
       <c r="C25" s="7"/>
       <c r="D25" s="8"/>
-      <c r="E25" s="8" t="n">
-        <v>2</v>
-      </c>
+      <c r="E25" s="8"/>
       <c r="F25" s="8"/>
-      <c r="G25" s="8" t="n">
-        <f aca="false">E25-F25</f>
-        <v>2</v>
-      </c>
-      <c r="H25" s="9" t="n">
-        <f aca="false">(F25/(F25+G25))</f>
-        <v>0</v>
-      </c>
+      <c r="G25" s="8"/>
+      <c r="H25" s="9"/>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>35</v>
-      </c>
+      <c r="A26" s="6"/>
+      <c r="B26" s="6"/>
       <c r="C26" s="7"/>
       <c r="D26" s="8"/>
-      <c r="E26" s="8" t="n">
-        <v>2</v>
-      </c>
+      <c r="E26" s="8"/>
       <c r="F26" s="8"/>
-      <c r="G26" s="8" t="n">
-        <f aca="false">E26-F26</f>
-        <v>2</v>
-      </c>
-      <c r="H26" s="9" t="n">
-        <f aca="false">(F26/(F26+G26))</f>
-        <v>0</v>
-      </c>
+      <c r="G26" s="8"/>
+      <c r="H26" s="9"/>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>36</v>
-      </c>
+      <c r="A27" s="6"/>
+      <c r="B27" s="6"/>
       <c r="C27" s="7"/>
       <c r="D27" s="8"/>
-      <c r="E27" s="8" t="n">
-        <v>2</v>
-      </c>
+      <c r="E27" s="8"/>
       <c r="F27" s="8"/>
-      <c r="G27" s="8" t="n">
-        <f aca="false">E27-F27</f>
-        <v>2</v>
-      </c>
-      <c r="H27" s="9" t="n">
-        <f aca="false">(F27/(F27+G27))</f>
-        <v>0</v>
-      </c>
+      <c r="G27" s="8"/>
+      <c r="H27" s="9"/>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>37</v>
-      </c>
+      <c r="A28" s="6"/>
+      <c r="B28" s="6"/>
       <c r="C28" s="7"/>
       <c r="D28" s="8"/>
-      <c r="E28" s="8" t="n">
-        <v>2</v>
-      </c>
+      <c r="E28" s="8"/>
       <c r="F28" s="8"/>
-      <c r="G28" s="8" t="n">
-        <f aca="false">E28-F28</f>
-        <v>2</v>
-      </c>
-      <c r="H28" s="9" t="n">
-        <f aca="false">(F28/(F28+G28))</f>
-        <v>0</v>
-      </c>
+      <c r="G28" s="8"/>
+      <c r="H28" s="9"/>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>38</v>
-      </c>
+      <c r="A29" s="6"/>
+      <c r="B29" s="6"/>
       <c r="C29" s="7"/>
       <c r="D29" s="8"/>
-      <c r="E29" s="8" t="n">
-        <v>2</v>
-      </c>
+      <c r="E29" s="8"/>
       <c r="F29" s="8"/>
-      <c r="G29" s="8" t="n">
-        <f aca="false">E29-F29</f>
-        <v>2</v>
-      </c>
-      <c r="H29" s="9" t="n">
-        <f aca="false">(F29/(F29+G29))</f>
-        <v>0</v>
-      </c>
+      <c r="G29" s="8"/>
+      <c r="H29" s="9"/>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>39</v>
-      </c>
+      <c r="A30" s="6"/>
+      <c r="B30" s="6"/>
       <c r="C30" s="7"/>
       <c r="D30" s="8"/>
-      <c r="E30" s="8" t="n">
-        <v>2</v>
-      </c>
+      <c r="E30" s="8"/>
       <c r="F30" s="8"/>
-      <c r="G30" s="8" t="n">
-        <f aca="false">E30-F30</f>
-        <v>2</v>
-      </c>
-      <c r="H30" s="9" t="n">
-        <f aca="false">(F30/(F30+G30))</f>
-        <v>0</v>
-      </c>
+      <c r="G30" s="8"/>
+      <c r="H30" s="9"/>
     </row>
     <row r="31" customFormat="false" ht="26.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B31" s="6" t="s">
-        <v>40</v>
-      </c>
+      <c r="A31" s="6"/>
+      <c r="B31" s="6"/>
       <c r="C31" s="7"/>
       <c r="D31" s="8"/>
-      <c r="E31" s="8" t="n">
-        <v>2</v>
-      </c>
+      <c r="E31" s="8"/>
       <c r="F31" s="8"/>
-      <c r="G31" s="8" t="n">
-        <f aca="false">E31-F31</f>
-        <v>2</v>
-      </c>
-      <c r="H31" s="9" t="n">
-        <f aca="false">(F31/(F31+G31))</f>
-        <v>0</v>
-      </c>
+      <c r="G31" s="8"/>
+      <c r="H31" s="9"/>
     </row>
     <row r="32" customFormat="false" ht="28.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>41</v>
-      </c>
+      <c r="A32" s="6"/>
+      <c r="B32" s="6"/>
       <c r="C32" s="7"/>
       <c r="D32" s="8"/>
-      <c r="E32" s="8" t="n">
-        <v>2</v>
-      </c>
+      <c r="E32" s="8"/>
       <c r="F32" s="8"/>
-      <c r="G32" s="8" t="n">
-        <f aca="false">E32-F32</f>
-        <v>2</v>
-      </c>
-      <c r="H32" s="9" t="n">
-        <f aca="false">(F32/(F32+G32))</f>
-        <v>0</v>
-      </c>
+      <c r="G32" s="8"/>
+      <c r="H32" s="9"/>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="6" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="C33" s="7"/>
       <c r="D33" s="8"/>
@@ -1251,7 +1104,7 @@
     <row r="34" customFormat="false" ht="27.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="6"/>
       <c r="B34" s="8" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C34" s="8"/>
       <c r="D34" s="8"/>
@@ -1271,7 +1124,7 @@
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="6"/>
       <c r="B35" s="6" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="C35" s="8"/>
       <c r="D35" s="8"/>
@@ -1295,7 +1148,7 @@
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="6"/>
       <c r="B36" s="8" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="C36" s="8"/>
       <c r="D36" s="8"/>
@@ -1315,7 +1168,7 @@
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="6"/>
       <c r="B37" s="6" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="C37" s="8"/>
       <c r="D37" s="8"/>
@@ -1334,10 +1187,10 @@
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="6" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="C38" s="8"/>
       <c r="D38" s="8"/>
@@ -1361,7 +1214,7 @@
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="6"/>
       <c r="B39" s="6" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C39" s="8"/>
       <c r="D39" s="8"/>
@@ -1381,7 +1234,7 @@
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="6"/>
       <c r="B40" s="8" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="C40" s="8"/>
       <c r="D40" s="8"/>
@@ -1401,7 +1254,7 @@
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="6"/>
       <c r="B41" s="6" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="C41" s="8"/>
       <c r="D41" s="8"/>
@@ -1425,7 +1278,7 @@
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="6"/>
       <c r="B42" s="6" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="C42" s="8"/>
       <c r="D42" s="8"/>
@@ -1445,7 +1298,7 @@
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="6"/>
       <c r="B43" s="6" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="C43" s="8"/>
       <c r="D43" s="8"/>
@@ -1465,7 +1318,7 @@
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="6"/>
       <c r="B44" s="6" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="C44" s="8"/>
       <c r="D44" s="8"/>
@@ -1489,7 +1342,7 @@
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="6"/>
       <c r="B45" s="6" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="C45" s="8"/>
       <c r="D45" s="8"/>
@@ -1508,10 +1361,10 @@
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="6" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="C46" s="8"/>
       <c r="D46" s="8"/>
@@ -1535,7 +1388,7 @@
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="6"/>
       <c r="B47" s="6" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C47" s="8"/>
       <c r="D47" s="8"/>
@@ -1555,7 +1408,7 @@
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="6"/>
       <c r="B48" s="6" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="C48" s="8"/>
       <c r="D48" s="8"/>
@@ -1575,7 +1428,7 @@
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="6"/>
       <c r="B49" s="6" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="C49" s="8"/>
       <c r="D49" s="8"/>
@@ -1599,7 +1452,7 @@
     <row r="50" customFormat="false" ht="31.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="6"/>
       <c r="B50" s="6" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="C50" s="8"/>
       <c r="D50" s="8"/>
@@ -1619,7 +1472,7 @@
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="6"/>
       <c r="B51" s="6" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="C51" s="8"/>
       <c r="D51" s="8"/>
@@ -1641,7 +1494,7 @@
         <v>10</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="C52" s="8"/>
       <c r="D52" s="8"/>
@@ -1661,7 +1514,7 @@
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="6"/>
       <c r="B53" s="8" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="C53" s="8"/>
       <c r="D53" s="8"/>
@@ -1680,10 +1533,10 @@
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="6" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="C54" s="8"/>
       <c r="D54" s="8"/>
@@ -1703,7 +1556,7 @@
     <row r="55" customFormat="false" ht="29.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="8"/>
       <c r="B55" s="8" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="C55" s="8"/>
       <c r="D55" s="8"/>
@@ -1727,7 +1580,7 @@
     <row r="56" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="8"/>
       <c r="B56" s="8" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C56" s="8"/>
       <c r="D56" s="8"/>
@@ -1747,7 +1600,7 @@
     <row r="57" customFormat="false" ht="28.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="8"/>
       <c r="B57" s="6" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="C57" s="8"/>
       <c r="D57" s="8"/>
@@ -1771,7 +1624,7 @@
     <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="6"/>
       <c r="B58" s="8" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="C58" s="8"/>
       <c r="D58" s="8"/>
@@ -1791,7 +1644,7 @@
     <row r="59" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="6"/>
       <c r="B59" s="6" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="C59" s="8"/>
       <c r="D59" s="8"/>
@@ -1810,10 +1663,10 @@
     </row>
     <row r="60" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="6" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="B60" s="8" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="C60" s="8"/>
       <c r="D60" s="8"/>
@@ -1833,7 +1686,7 @@
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="8"/>
       <c r="B61" s="6" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="C61" s="8"/>
       <c r="D61" s="8"/>
@@ -1857,7 +1710,7 @@
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="6"/>
       <c r="B62" s="6" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C62" s="8"/>
       <c r="D62" s="8"/>
@@ -1877,7 +1730,7 @@
     <row r="63" customFormat="false" ht="30.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="6"/>
       <c r="B63" s="8" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="C63" s="8"/>
       <c r="D63" s="8"/>
@@ -1897,7 +1750,7 @@
     <row r="64" customFormat="false" ht="31.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="6"/>
       <c r="B64" s="6" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="C64" s="8"/>
       <c r="D64" s="8"/>
@@ -1921,7 +1774,7 @@
     <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="6"/>
       <c r="B65" s="6" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="C65" s="8"/>
       <c r="D65" s="8"/>
@@ -1941,7 +1794,7 @@
     <row r="66" customFormat="false" ht="26.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="6"/>
       <c r="B66" s="6" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="C66" s="8"/>
       <c r="D66" s="8"/>
@@ -1961,7 +1814,7 @@
     <row r="67" customFormat="false" ht="28.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="6"/>
       <c r="B67" s="6" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="C67" s="8"/>
       <c r="D67" s="8"/>
@@ -1985,7 +1838,7 @@
     <row r="68" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="6"/>
       <c r="B68" s="6" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="C68" s="8"/>
       <c r="D68" s="8"/>
@@ -2004,10 +1857,10 @@
     </row>
     <row r="69" customFormat="false" ht="40.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="6" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="C69" s="8"/>
       <c r="D69" s="8"/>
@@ -2027,7 +1880,7 @@
     <row r="70" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="8"/>
       <c r="B70" s="6" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="C70" s="8"/>
       <c r="D70" s="8"/>
@@ -2051,7 +1904,7 @@
     <row r="71" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="6"/>
       <c r="B71" s="6" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C71" s="8"/>
       <c r="D71" s="8"/>
@@ -2071,7 +1924,7 @@
     <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="6"/>
       <c r="B72" s="6" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="C72" s="8"/>
       <c r="D72" s="8"/>
@@ -2091,7 +1944,7 @@
     <row r="73" customFormat="false" ht="40.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="6"/>
       <c r="B73" s="6" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="C73" s="8"/>
       <c r="D73" s="8"/>
@@ -2115,7 +1968,7 @@
     <row r="74" customFormat="false" ht="28.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="6"/>
       <c r="B74" s="6" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="C74" s="8"/>
       <c r="D74" s="8"/>
@@ -2135,7 +1988,7 @@
     <row r="75" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="6"/>
       <c r="B75" s="6" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="C75" s="8"/>
       <c r="D75" s="8"/>
@@ -2154,10 +2007,10 @@
     </row>
     <row r="76" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="6" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="B76" s="6" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="C76" s="8"/>
       <c r="D76" s="8"/>
@@ -2177,7 +2030,7 @@
     <row r="77" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="6"/>
       <c r="B77" s="6" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="C77" s="8"/>
       <c r="D77" s="8"/>
@@ -2197,7 +2050,7 @@
     <row r="78" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="6"/>
       <c r="B78" s="6" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="C78" s="8"/>
       <c r="D78" s="8"/>
@@ -2217,7 +2070,7 @@
     <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="6"/>
       <c r="B79" s="6" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="C79" s="8"/>
       <c r="D79" s="8"/>
@@ -2236,10 +2089,10 @@
     </row>
     <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="6" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="B80" s="6" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="C80" s="8"/>
       <c r="D80" s="8"/>
@@ -2259,7 +2112,7 @@
     <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="6"/>
       <c r="B81" s="8" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="C81" s="8"/>
       <c r="D81" s="8"/>
@@ -2279,7 +2132,7 @@
     <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="6"/>
       <c r="B82" s="6" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="C82" s="8"/>
       <c r="D82" s="8"/>
@@ -2299,7 +2152,7 @@
     <row r="83" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="6"/>
       <c r="B83" s="6" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C83" s="8"/>
       <c r="D83" s="8"/>
@@ -2318,10 +2171,10 @@
     </row>
     <row r="84" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="6" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="B84" s="6" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="C84" s="8"/>
       <c r="D84" s="8"/>
@@ -2341,7 +2194,7 @@
     <row r="85" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A85" s="6"/>
       <c r="B85" s="8" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="C85" s="8"/>
       <c r="D85" s="8"/>
@@ -2361,7 +2214,7 @@
     <row r="86" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A86" s="6"/>
       <c r="B86" s="6" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="C86" s="8"/>
       <c r="D86" s="8"/>
@@ -2381,7 +2234,7 @@
     <row r="87" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A87" s="6"/>
       <c r="B87" s="6" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="C87" s="8"/>
       <c r="D87" s="8"/>
@@ -2400,10 +2253,10 @@
     </row>
     <row r="88" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A88" s="6" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="C88" s="8"/>
       <c r="D88" s="8"/>
@@ -2423,7 +2276,7 @@
     <row r="89" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A89" s="6"/>
       <c r="B89" s="6" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="C89" s="8"/>
       <c r="D89" s="8"/>
@@ -2443,7 +2296,7 @@
     <row r="90" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A90" s="6"/>
       <c r="B90" s="6" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="C90" s="8"/>
       <c r="D90" s="8"/>
@@ -2463,7 +2316,7 @@
     <row r="91" customFormat="false" ht="29.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A91" s="6"/>
       <c r="B91" s="6" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="C91" s="8"/>
       <c r="D91" s="8"/>
@@ -2483,7 +2336,7 @@
     <row r="92" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A92" s="6"/>
       <c r="B92" s="6" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="C92" s="8"/>
       <c r="D92" s="8"/>
@@ -2502,10 +2355,10 @@
     </row>
     <row r="93" customFormat="false" ht="27.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A93" s="6" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="B93" s="6" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="C93" s="8"/>
       <c r="D93" s="8"/>
@@ -2525,7 +2378,7 @@
     <row r="94" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A94" s="6"/>
       <c r="B94" s="6" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="C94" s="8"/>
       <c r="D94" s="8"/>
@@ -2545,7 +2398,7 @@
     <row r="95" customFormat="false" ht="30.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A95" s="6"/>
       <c r="B95" s="8" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="C95" s="8"/>
       <c r="D95" s="8"/>
@@ -2565,7 +2418,7 @@
     <row r="96" customFormat="false" ht="26.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A96" s="6"/>
       <c r="B96" s="6" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="C96" s="8"/>
       <c r="D96" s="8"/>
@@ -2585,7 +2438,7 @@
     <row r="97" customFormat="false" ht="29.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A97" s="6"/>
       <c r="B97" s="6" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C97" s="8"/>
       <c r="D97" s="8"/>
@@ -2604,10 +2457,10 @@
     </row>
     <row r="98" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A98" s="6" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="B98" s="6" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="C98" s="8"/>
       <c r="D98" s="8"/>
@@ -2627,7 +2480,7 @@
     <row r="99" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A99" s="6"/>
       <c r="B99" s="6" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="C99" s="8"/>
       <c r="D99" s="8"/>
@@ -2647,7 +2500,7 @@
     <row r="100" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A100" s="6"/>
       <c r="B100" s="8" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="C100" s="8"/>
       <c r="D100" s="8"/>
@@ -2667,7 +2520,7 @@
     <row r="101" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A101" s="6"/>
       <c r="B101" s="6" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="C101" s="8"/>
       <c r="D101" s="8"/>
@@ -2687,7 +2540,7 @@
     <row r="102" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A102" s="6"/>
       <c r="B102" s="6" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="C102" s="8"/>
       <c r="D102" s="8"/>
@@ -2706,10 +2559,10 @@
     </row>
     <row r="103" customFormat="false" ht="27.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A103" s="6" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="B103" s="6" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="C103" s="8"/>
       <c r="D103" s="8"/>
@@ -2729,7 +2582,7 @@
     <row r="104" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A104" s="6"/>
       <c r="B104" s="6" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="C104" s="8"/>
       <c r="D104" s="8"/>
@@ -2747,45 +2600,39 @@
       </c>
     </row>
     <row r="105" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A105" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="B105" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="C105" s="8"/>
-      <c r="D105" s="8"/>
-      <c r="E105" s="8" t="n">
-        <f aca="false">SUM(E106:E107)</f>
-        <v>4</v>
-      </c>
-      <c r="F105" s="8" t="n">
-        <f aca="false">SUM(F106:F107)</f>
-        <v>0</v>
-      </c>
-      <c r="G105" s="8" t="n">
-        <f aca="false">SUM(G106:G107)</f>
-        <v>4</v>
-      </c>
-      <c r="H105" s="9" t="n">
-        <f aca="false">(F105/(F105+G105))</f>
-        <v>0</v>
-      </c>
+      <c r="A105" s="0"/>
+      <c r="B105" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C105" s="0"/>
+      <c r="D105" s="0"/>
+      <c r="E105" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="F105" s="0"/>
+      <c r="G105" s="0"/>
+      <c r="H105" s="0"/>
     </row>
     <row r="106" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A106" s="6"/>
+      <c r="A106" s="6" t="s">
+        <v>32</v>
+      </c>
       <c r="B106" s="6" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="C106" s="8"/>
       <c r="D106" s="8"/>
       <c r="E106" s="8" t="n">
-        <v>2</v>
-      </c>
-      <c r="F106" s="8"/>
+        <f aca="false">SUM(E107:E108)</f>
+        <v>4</v>
+      </c>
+      <c r="F106" s="8" t="n">
+        <f aca="false">SUM(F107:F108)</f>
+        <v>0</v>
+      </c>
       <c r="G106" s="8" t="n">
-        <f aca="false">E106-F106</f>
-        <v>2</v>
+        <f aca="false">SUM(G107:G108)</f>
+        <v>4</v>
       </c>
       <c r="H106" s="9" t="n">
         <f aca="false">(F106/(F106+G106))</f>
@@ -2795,7 +2642,7 @@
     <row r="107" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A107" s="6"/>
       <c r="B107" s="6" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="C107" s="8"/>
       <c r="D107" s="8"/>
@@ -2813,21 +2660,19 @@
       </c>
     </row>
     <row r="108" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A108" s="6" t="s">
-        <v>64</v>
-      </c>
+      <c r="A108" s="6"/>
       <c r="B108" s="6" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="C108" s="8"/>
       <c r="D108" s="8"/>
       <c r="E108" s="8" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F108" s="8"/>
       <c r="G108" s="8" t="n">
         <f aca="false">E108-F108</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H108" s="9" t="n">
         <f aca="false">(F108/(F108+G108))</f>
@@ -2836,24 +2681,20 @@
     </row>
     <row r="109" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A109" s="6" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B109" s="6" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C109" s="8"/>
       <c r="D109" s="8"/>
       <c r="E109" s="8" t="n">
-        <f aca="false">SUM(E110:E111)</f>
-        <v>10</v>
-      </c>
-      <c r="F109" s="8" t="n">
-        <f aca="false">SUM(F110:F111)</f>
-        <v>0</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F109" s="8"/>
       <c r="G109" s="8" t="n">
-        <f aca="false">SUM(G110:G111)</f>
-        <v>10</v>
+        <f aca="false">E109-F109</f>
+        <v>5</v>
       </c>
       <c r="H109" s="9" t="n">
         <f aca="false">(F109/(F109+G109))</f>
@@ -2861,19 +2702,25 @@
       </c>
     </row>
     <row r="110" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A110" s="7"/>
+      <c r="A110" s="6" t="s">
+        <v>50</v>
+      </c>
       <c r="B110" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="C110" s="7"/>
-      <c r="D110" s="7"/>
-      <c r="E110" s="7" t="n">
-        <v>5</v>
-      </c>
-      <c r="F110" s="8"/>
+        <v>73</v>
+      </c>
+      <c r="C110" s="8"/>
+      <c r="D110" s="8"/>
+      <c r="E110" s="8" t="n">
+        <f aca="false">SUM(E111:E112)</f>
+        <v>10</v>
+      </c>
+      <c r="F110" s="8" t="n">
+        <f aca="false">SUM(F111:F112)</f>
+        <v>0</v>
+      </c>
       <c r="G110" s="8" t="n">
-        <f aca="false">E110-F110</f>
-        <v>5</v>
+        <f aca="false">SUM(G111:G112)</f>
+        <v>10</v>
       </c>
       <c r="H110" s="9" t="n">
         <f aca="false">(F110/(F110+G110))</f>
@@ -2883,14 +2730,14 @@
     <row r="111" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A111" s="7"/>
       <c r="B111" s="6" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="C111" s="7"/>
       <c r="D111" s="7"/>
       <c r="E111" s="7" t="n">
         <v>5</v>
       </c>
-      <c r="F111" s="7"/>
+      <c r="F111" s="8"/>
       <c r="G111" s="8" t="n">
         <f aca="false">E111-F111</f>
         <v>5</v>
@@ -2901,21 +2748,19 @@
       </c>
     </row>
     <row r="112" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A112" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="B112" s="7" t="s">
-        <v>85</v>
+      <c r="A112" s="7"/>
+      <c r="B112" s="6" t="s">
+        <v>75</v>
       </c>
       <c r="C112" s="7"/>
       <c r="D112" s="7"/>
       <c r="E112" s="7" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F112" s="7"/>
       <c r="G112" s="8" t="n">
         <f aca="false">E112-F112</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H112" s="9" t="n">
         <f aca="false">(F112/(F112+G112))</f>
@@ -2923,14 +2768,26 @@
       </c>
     </row>
     <row r="113" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A113" s="0"/>
-      <c r="B113" s="0"/>
-      <c r="C113" s="0"/>
-      <c r="D113" s="0"/>
-      <c r="E113" s="0"/>
-      <c r="F113" s="0"/>
-      <c r="G113" s="0"/>
-      <c r="H113" s="0"/>
+      <c r="A113" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B113" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C113" s="7"/>
+      <c r="D113" s="7"/>
+      <c r="E113" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="F113" s="7"/>
+      <c r="G113" s="8" t="n">
+        <f aca="false">E113-F113</f>
+        <v>2</v>
+      </c>
+      <c r="H113" s="9" t="n">
+        <f aca="false">(F113/(F113+G113))</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="114" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A114" s="0"/>
@@ -2959,7 +2816,7 @@
       <c r="D116" s="0"/>
       <c r="E116" s="8" t="n">
         <f aca="false">SUM(E4:E112)</f>
-        <v>390</v>
+        <v>378</v>
       </c>
       <c r="F116" s="8" t="n">
         <f aca="false">SUM(F4:F112)</f>
@@ -2967,11 +2824,11 @@
       </c>
       <c r="G116" s="8" t="n">
         <f aca="false">SUM(G4:G112)</f>
-        <v>348</v>
+        <v>326</v>
       </c>
       <c r="H116" s="9" t="n">
         <f aca="false">(F116/(F116+G116))</f>
-        <v>0.107692307692308</v>
+        <v>0.114130434782609</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2983,7 +2840,7 @@
     </row>
     <row r="118" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A118" s="10" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="B118" s="2"/>
     </row>
@@ -2992,17 +2849,17 @@
     </row>
     <row r="120" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A120" s="3" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="B120" s="2"/>
     </row>
     <row r="121" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A121" s="11" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="B121" s="12" t="n">
         <f aca="false">Feuil1!E116</f>
-        <v>390</v>
+        <v>378</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3020,12 +2877,12 @@
       </c>
       <c r="B123" s="12" t="n">
         <f aca="false">Feuil1!G116</f>
-        <v>348</v>
+        <v>326</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B124" s="12" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>